<commit_message>
Avance de la actualizacion de la fecha entrada/salida socio
</commit_message>
<xml_diff>
--- a/CentroDeportivo/DDBB/IPS BD RELACIONAL.xlsx
+++ b/CentroDeportivo/DDBB/IPS BD RELACIONAL.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="63">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>SOCIO</t>
+  </si>
+  <si>
+    <t>HORA_IENTRADA</t>
+  </si>
+  <si>
+    <t>HORA_SALIDA</t>
   </si>
 </sst>
 </file>
@@ -374,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -402,14 +408,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -435,6 +435,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:K46"/>
+  <dimension ref="A5:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I17" sqref="G16:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -727,16 +740,16 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:11">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="29"/>
-      <c r="G5" s="30" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="38"/>
+      <c r="G5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="32"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="30"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
@@ -891,10 +904,10 @@
       <c r="I13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="36" t="s">
+      <c r="J13" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="37"/>
+      <c r="K13" s="35"/>
     </row>
     <row r="14" spans="1:11">
       <c r="G14" s="12" t="s">
@@ -906,331 +919,318 @@
       <c r="I14" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="36"/>
-      <c r="K14" s="37"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="35"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="H15" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" s="25" t="s">
+      <c r="H15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="36"/>
-      <c r="K15" s="37"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="B17" s="30" t="s">
+      <c r="J15" s="34"/>
+      <c r="K15" s="35"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="G16" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="42"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1">
+      <c r="G17" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="41"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1"/>
+    <row r="19" spans="1:11">
+      <c r="B19" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
-      <c r="G17" s="30" t="s">
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
+      <c r="G19" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="31"/>
-      <c r="I17" s="32"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" t="s">
+      <c r="H19" s="29"/>
+      <c r="I19" s="30"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="C20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="B19" s="5" t="s">
+      <c r="H20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="B21" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G19" s="5" t="s">
+      <c r="C21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="B20" s="5" t="s">
+      <c r="H21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="B22" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="G20" s="16" t="s">
+      <c r="C22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="G22" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" s="11"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="B21" s="5" t="s">
+      <c r="H22" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="B23" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="B22" s="16" t="s">
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="B24" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C24" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="G24" s="27" t="s">
+      <c r="D24" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="G26" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="H24" s="28"/>
-      <c r="I24" s="29"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="B25" s="30" t="s">
+      <c r="H26" s="37"/>
+      <c r="I26" s="38"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="B27" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="32"/>
-      <c r="F25" t="s">
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
+      <c r="F27" t="s">
         <v>2</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" t="s">
+      <c r="H27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G26" s="5" t="s">
+      <c r="C28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="B27" s="5" t="s">
+      <c r="H28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="B29" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="G27" s="5" t="s">
+      <c r="C29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="G29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="B28" s="5" t="s">
+      <c r="H29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="B30" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="G28" s="5" t="s">
+      <c r="D30" s="7"/>
+      <c r="G30" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H30" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I28" s="7"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="B29" s="5" t="s">
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="B31" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G29" s="5" t="s">
+      <c r="D31" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="H31" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I29" s="7"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="B30" s="5" t="s">
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="B32" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G30" s="5" t="s">
+      <c r="C32" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="H32" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="7"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="B31" s="16" t="s">
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="B33" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G31" s="18" t="s">
+      <c r="C33" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="H33" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I31" s="24" t="s">
+      <c r="I33" s="24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
-      <c r="G32" s="5" t="s">
+    <row r="34" spans="1:9">
+      <c r="G34" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H32" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I32" s="7" t="s">
+      <c r="H34" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I34" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
-      <c r="G33" s="9" t="s">
+    <row r="35" spans="1:9">
+      <c r="G35" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="H35" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I33" s="11"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="B34" s="30" t="s">
+      <c r="I35" s="11"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="B36" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="32"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" t="s">
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B37" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="B36" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G36" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="H36" s="34"/>
-      <c r="I36" s="35"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="B37" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="C37" s="6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>5</v>
-      </c>
-      <c r="G37" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="H37" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="I37" s="26" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="B38" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>8</v>
@@ -1238,127 +1238,163 @@
       <c r="D38" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G38" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I38" s="25" t="s">
-        <v>33</v>
-      </c>
+      <c r="G38" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="H38" s="32"/>
+      <c r="I38" s="33"/>
     </row>
     <row r="39" spans="1:9">
       <c r="B39" s="5" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="7"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
+      <c r="D39" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I39" s="26" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="40" spans="1:9">
       <c r="B40" s="5" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="7"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="23"/>
+      <c r="D40" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I40" s="25" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="41" spans="1:9">
       <c r="B41" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D41" s="7"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="23"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
     </row>
     <row r="42" spans="1:9">
       <c r="B42" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="B43" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="B44" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" s="7"/>
-      <c r="G42" s="33" t="s">
+      <c r="C44" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="G44" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="H42" s="34"/>
-      <c r="I42" s="35"/>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="B43" s="16" t="s">
+      <c r="H44" s="32"/>
+      <c r="I44" s="33"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="B45" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C45" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D43" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G43" s="19" t="s">
+      <c r="D45" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H43" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="I43" s="26" t="s">
+      <c r="H45" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I45" s="26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
-      <c r="G44" s="18" t="s">
+    <row r="46" spans="1:9">
+      <c r="G46" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H44" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="I44" s="24" t="s">
+      <c r="H46" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I46" s="24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
-      <c r="G45" s="21" t="s">
+    <row r="47" spans="1:9">
+      <c r="G47" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H45" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I45" s="25" t="s">
+      <c r="H47" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I47" s="25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
-      <c r="G46" s="23"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="23"/>
+    <row r="48" spans="1:9">
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="J13:K15"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="G5:I5"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="J13:K15"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modificado baja a DATE, añadida comprobacion de socio dado de baja
</commit_message>
<xml_diff>
--- a/CentroDeportivo/DDBB/IPS BD RELACIONAL.xlsx
+++ b/CentroDeportivo/DDBB/IPS BD RELACIONAL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uo244965\Downloads\proyecto\IPS\CentroDeportivo\DDBB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Carla\Documents\Git\Temp\ips\IPS\CentroDeportivo\DDBB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="65">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>HORA_SALIDA</t>
+  </si>
+  <si>
+    <t>FECHA_BAJA</t>
   </si>
 </sst>
 </file>
@@ -426,6 +429,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -450,18 +465,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,32 +742,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43:D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.375" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.375" customWidth="1"/>
+    <col min="7" max="7" width="18.375" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.375" customWidth="1"/>
+    <col min="10" max="10" width="18.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:11">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="37"/>
-      <c r="G5" s="27" t="s">
+      <c r="C5" s="31"/>
+      <c r="D5" s="32"/>
+      <c r="G5" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="29"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="35"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
@@ -919,10 +922,10 @@
       <c r="I13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="33" t="s">
+      <c r="J13" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="34"/>
+      <c r="K13" s="40"/>
     </row>
     <row r="14" spans="1:11">
       <c r="G14" s="12" t="s">
@@ -934,8 +937,8 @@
       <c r="I14" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="33"/>
-      <c r="K14" s="34"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="40"/>
     </row>
     <row r="15" spans="1:11">
       <c r="G15" s="14" t="s">
@@ -947,27 +950,27 @@
       <c r="I15" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="33"/>
-      <c r="K15" s="34"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="40"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1">
-      <c r="G16" s="39" t="s">
+      <c r="G16" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="H16" s="28" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="G17" s="39" t="s">
+      <c r="C17" s="34"/>
+      <c r="D17" s="35"/>
+      <c r="G17" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="H17" s="39" t="s">
+      <c r="H17" s="28" t="s">
         <v>10</v>
       </c>
     </row>
@@ -995,11 +998,11 @@
       <c r="D19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="H19" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="29"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="35"/>
     </row>
     <row r="20" spans="1:10">
       <c r="B20" s="5" t="s">
@@ -1058,11 +1061,11 @@
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="25" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="29"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="35"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" thickBot="1">
       <c r="A26" t="s">
@@ -1077,11 +1080,11 @@
       <c r="D26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="35" t="s">
+      <c r="H26" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="I26" s="36"/>
-      <c r="J26" s="37"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="32"/>
     </row>
     <row r="27" spans="1:10">
       <c r="B27" s="5" t="s">
@@ -1197,11 +1200,11 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="29"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="35"/>
       <c r="H34" s="5" t="s">
         <v>25</v>
       </c>
@@ -1265,11 +1268,11 @@
       <c r="D38" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H38" s="30" t="s">
+      <c r="H38" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="I38" s="31"/>
-      <c r="J38" s="32"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="38"/>
     </row>
     <row r="39" spans="1:10">
       <c r="B39" s="5" t="s">
@@ -1279,7 +1282,7 @@
         <v>8</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="F39" s="40"/>
+      <c r="F39" s="29"/>
       <c r="H39" s="19" t="s">
         <v>29</v>
       </c>
@@ -1316,10 +1319,10 @@
         <v>8</v>
       </c>
       <c r="D41" s="7"/>
-      <c r="H41" s="38" t="s">
+      <c r="H41" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="I41" s="38" t="s">
+      <c r="I41" s="27" t="s">
         <v>24</v>
       </c>
       <c r="J41" s="22"/>
@@ -1337,13 +1340,14 @@
       <c r="J42" s="23"/>
     </row>
     <row r="43" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B43" s="16" t="s">
+      <c r="A43" s="7"/>
+      <c r="B43" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="7" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="23"/>
@@ -1351,11 +1355,19 @@
       <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10" ht="15.75" thickBot="1">
-      <c r="H44" s="30" t="s">
+      <c r="A44" s="7"/>
+      <c r="B44" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="11"/>
+      <c r="H44" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="I44" s="31"/>
-      <c r="J44" s="32"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="38"/>
     </row>
     <row r="45" spans="1:10">
       <c r="H45" s="19" t="s">
@@ -1392,16 +1404,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="J13:K15"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="H19:J19"/>
     <mergeCell ref="H26:J26"/>
     <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="H38:J38"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="J13:K15"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
CapaInterfaz.Monitor, nuevas clases Actividad, Curso, Monitor, MonitorDatos
</commit_message>
<xml_diff>
--- a/CentroDeportivo/DDBB/IPS BD RELACIONAL.xlsx
+++ b/CentroDeportivo/DDBB/IPS BD RELACIONAL.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uo244965\Downloads\proyecto\IPS\CentroDeportivo\DDBB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nacho\Documents\GitHub\IPS\IPS\CentroDeportivo\DDBB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22950" windowHeight="10200"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22956" windowHeight="10200"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="65">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -211,18 +211,28 @@
   </si>
   <si>
     <t>HORA_SALIDA</t>
+  </si>
+  <si>
+    <t>FECHA_BAJA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -260,6 +270,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -269,7 +285,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -394,11 +410,87 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -407,25 +499,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -435,19 +528,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -459,9 +552,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,32 +839,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:11">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="37"/>
-      <c r="G5" s="27" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="38"/>
+      <c r="G5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="30"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
@@ -919,10 +1019,10 @@
       <c r="I13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="33" t="s">
+      <c r="J13" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="34"/>
+      <c r="K13" s="35"/>
     </row>
     <row r="14" spans="1:11">
       <c r="G14" s="12" t="s">
@@ -931,11 +1031,11 @@
       <c r="H14" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="I14" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="33"/>
-      <c r="K14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="35"/>
     </row>
     <row r="15" spans="1:11">
       <c r="G15" s="14" t="s">
@@ -944,34 +1044,34 @@
       <c r="H15" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="25" t="s">
+      <c r="I15" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="33"/>
-      <c r="K15" s="34"/>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
-      <c r="G16" s="39" t="s">
+      <c r="J15" s="34"/>
+      <c r="K15" s="35"/>
+    </row>
+    <row r="16" spans="1:11" ht="15" thickBot="1">
+      <c r="G16" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="H16" s="26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B17" s="27" t="s">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
+      <c r="B17" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="G17" s="39" t="s">
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="G17" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="H17" s="39" t="s">
+      <c r="H17" s="26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -985,7 +1085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="B19" s="5" t="s">
         <v>3</v>
       </c>
@@ -995,11 +1095,11 @@
       <c r="D19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="H19" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="B20" s="5" t="s">
@@ -1038,7 +1138,7 @@
       </c>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="B22" s="16" t="s">
         <v>40</v>
       </c>
@@ -1056,15 +1156,15 @@
       </c>
       <c r="J22" s="11"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B25" s="27" t="s">
+    <row r="24" spans="1:10" ht="15" thickBot="1"/>
+    <row r="25" spans="1:10" ht="15" thickBot="1">
+      <c r="B25" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="29"/>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1">
+      <c r="C25" s="29"/>
+      <c r="D25" s="30"/>
+    </row>
+    <row r="26" spans="1:10" ht="15" thickBot="1">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1077,11 +1177,11 @@
       <c r="D26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="35" t="s">
+      <c r="H26" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="I26" s="36"/>
-      <c r="J26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="38"/>
     </row>
     <row r="27" spans="1:10">
       <c r="B27" s="5" t="s">
@@ -1158,7 +1258,7 @@
       </c>
       <c r="J30" s="7"/>
     </row>
-    <row r="31" spans="1:10" ht="15.75" thickBot="1">
+    <row r="31" spans="1:10" ht="15" thickBot="1">
       <c r="B31" s="16" t="s">
         <v>48</v>
       </c>
@@ -1185,23 +1285,23 @@
       </c>
       <c r="J32" s="7"/>
     </row>
-    <row r="33" spans="1:10" ht="15.75" thickBot="1">
+    <row r="33" spans="1:10" ht="15" thickBot="1">
       <c r="H33" s="18" t="s">
         <v>49</v>
       </c>
       <c r="I33" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J33" s="24" t="s">
+      <c r="J33" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B34" s="27" t="s">
+    <row r="34" spans="1:10" ht="15" thickBot="1">
+      <c r="B34" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="30"/>
       <c r="H34" s="5" t="s">
         <v>25</v>
       </c>
@@ -1212,7 +1312,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" thickBot="1">
+    <row r="35" spans="1:10" ht="15" thickBot="1">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -1244,7 +1344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" thickBot="1">
+    <row r="37" spans="1:10" ht="15" thickBot="1">
       <c r="B37" s="5" t="s">
         <v>7</v>
       </c>
@@ -1255,7 +1355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" thickBot="1">
+    <row r="38" spans="1:10" ht="15" thickBot="1">
       <c r="B38" s="5" t="s">
         <v>38</v>
       </c>
@@ -1265,11 +1365,11 @@
       <c r="D38" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H38" s="30" t="s">
+      <c r="H38" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="I38" s="31"/>
-      <c r="J38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="33"/>
     </row>
     <row r="39" spans="1:10">
       <c r="B39" s="5" t="s">
@@ -1279,18 +1379,18 @@
         <v>8</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="F39" s="40"/>
+      <c r="F39" s="27"/>
       <c r="H39" s="19" t="s">
         <v>29</v>
       </c>
       <c r="I39" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="J39" s="26" t="s">
+      <c r="J39" s="25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" thickBot="1">
+    <row r="40" spans="1:10">
       <c r="B40" s="5" t="s">
         <v>56</v>
       </c>
@@ -1298,17 +1398,17 @@
         <v>8</v>
       </c>
       <c r="D40" s="7"/>
-      <c r="H40" s="21" t="s">
+      <c r="H40" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="I40" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J40" s="25" t="s">
+      <c r="I40" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="J40" s="41" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" ht="15" thickBot="1">
       <c r="B41" s="5" t="s">
         <v>57</v>
       </c>
@@ -1316,13 +1416,13 @@
         <v>8</v>
       </c>
       <c r="D41" s="7"/>
-      <c r="H41" s="38" t="s">
+      <c r="H41" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="I41" s="38" t="s">
+      <c r="I41" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="J41" s="22"/>
+      <c r="J41" s="44"/>
     </row>
     <row r="42" spans="1:10">
       <c r="B42" s="5" t="s">
@@ -1332,11 +1432,11 @@
         <v>8</v>
       </c>
       <c r="D42" s="7"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
-    </row>
-    <row r="43" spans="1:10" ht="15.75" thickBot="1">
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+    </row>
+    <row r="43" spans="1:10" ht="15" thickBot="1">
       <c r="B43" s="16" t="s">
         <v>60</v>
       </c>
@@ -1346,16 +1446,22 @@
       <c r="D43" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
-    </row>
-    <row r="44" spans="1:10" ht="15.75" thickBot="1">
-      <c r="H44" s="30" t="s">
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+    </row>
+    <row r="44" spans="1:10" ht="15" thickBot="1">
+      <c r="B44" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="H44" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="I44" s="31"/>
-      <c r="J44" s="32"/>
+      <c r="I44" s="32"/>
+      <c r="J44" s="33"/>
     </row>
     <row r="45" spans="1:10">
       <c r="H45" s="19" t="s">
@@ -1364,7 +1470,7 @@
       <c r="I45" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="J45" s="26" t="s">
+      <c r="J45" s="25" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1375,33 +1481,33 @@
       <c r="I46" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="J46" s="24" t="s">
+      <c r="J46" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15.75" thickBot="1">
+    <row r="47" spans="1:10" ht="15" thickBot="1">
       <c r="H47" s="21" t="s">
         <v>19</v>
       </c>
       <c r="I47" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J47" s="25" t="s">
+      <c r="J47" s="24" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="J13:K15"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="H19:J19"/>
     <mergeCell ref="H26:J26"/>
     <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="H38:J38"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="J13:K15"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
boton "Ver detalles" de Monitor
</commit_message>
<xml_diff>
--- a/CentroDeportivo/DDBB/IPS BD RELACIONAL.xlsx
+++ b/CentroDeportivo/DDBB/IPS BD RELACIONAL.xlsx
@@ -519,6 +519,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -528,13 +535,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -552,16 +562,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -855,16 +855,16 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:11">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
-      <c r="G5" s="28" t="s">
+      <c r="C5" s="45"/>
+      <c r="D5" s="46"/>
+      <c r="G5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="29"/>
-      <c r="I5" s="30"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="37"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
@@ -1019,10 +1019,10 @@
       <c r="I13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="34" t="s">
+      <c r="J13" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="35"/>
+      <c r="K13" s="43"/>
     </row>
     <row r="14" spans="1:11">
       <c r="G14" s="12" t="s">
@@ -1034,8 +1034,8 @@
       <c r="I14" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="34"/>
-      <c r="K14" s="35"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="43"/>
     </row>
     <row r="15" spans="1:11">
       <c r="G15" s="14" t="s">
@@ -1047,8 +1047,8 @@
       <c r="I15" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="34"/>
-      <c r="K15" s="35"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="43"/>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1">
       <c r="G16" s="26" t="s">
@@ -1059,11 +1059,11 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1">
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="37"/>
       <c r="G17" s="26" t="s">
         <v>63</v>
       </c>
@@ -1095,11 +1095,11 @@
       <c r="D19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="I19" s="29"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="B20" s="5" t="s">
@@ -1158,11 +1158,11 @@
     </row>
     <row r="24" spans="1:10" ht="15" thickBot="1"/>
     <row r="25" spans="1:10" ht="15" thickBot="1">
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="30"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="37"/>
     </row>
     <row r="26" spans="1:10" ht="15" thickBot="1">
       <c r="A26" t="s">
@@ -1177,11 +1177,11 @@
       <c r="D26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="36" t="s">
+      <c r="H26" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="I26" s="37"/>
-      <c r="J26" s="38"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="46"/>
     </row>
     <row r="27" spans="1:10">
       <c r="B27" s="5" t="s">
@@ -1297,11 +1297,11 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" thickBot="1">
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="30"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="37"/>
       <c r="H34" s="5" t="s">
         <v>25</v>
       </c>
@@ -1365,11 +1365,11 @@
       <c r="D38" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H38" s="45" t="s">
+      <c r="H38" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I38" s="32"/>
-      <c r="J38" s="33"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="40"/>
     </row>
     <row r="39" spans="1:10">
       <c r="B39" s="5" t="s">
@@ -1398,13 +1398,13 @@
         <v>8</v>
       </c>
       <c r="D40" s="7"/>
-      <c r="H40" s="39" t="s">
+      <c r="H40" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="I40" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="J40" s="41" t="s">
+      <c r="I40" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J40" s="30" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1416,13 +1416,13 @@
         <v>8</v>
       </c>
       <c r="D41" s="7"/>
-      <c r="H41" s="42" t="s">
+      <c r="H41" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="I41" s="43" t="s">
+      <c r="I41" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="J41" s="44"/>
+      <c r="J41" s="33"/>
     </row>
     <row r="42" spans="1:10">
       <c r="B42" s="5" t="s">
@@ -1451,17 +1451,17 @@
       <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10" ht="15" thickBot="1">
-      <c r="B44" s="46" t="s">
+      <c r="B44" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="46" t="s">
+      <c r="C44" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="H44" s="31" t="s">
+      <c r="H44" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="I44" s="32"/>
-      <c r="J44" s="33"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10">
       <c r="H45" s="19" t="s">

</xml_diff>

<commit_message>
añadida a la interfaz de monitor la seleccion de actividades dentro de un rango de fechas, falta asignar la hora
</commit_message>
<xml_diff>
--- a/CentroDeportivo/DDBB/IPS BD RELACIONAL.xlsx
+++ b/CentroDeportivo/DDBB/IPS BD RELACIONAL.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="66">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>FECHA_BAJA</t>
+  </si>
+  <si>
+    <t>FECHA_ACTIVIDAD</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -562,6 +565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1025,6 +1029,12 @@
       <c r="K13" s="43"/>
     </row>
     <row r="14" spans="1:11">
+      <c r="B14" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G14" s="12" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
excel sprint 3 de verdad
</commit_message>
<xml_diff>
--- a/CentroDeportivo/DDBB/IPS BD RELACIONAL.xlsx
+++ b/CentroDeportivo/DDBB/IPS BD RELACIONAL.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="70">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -217,18 +217,37 @@
   </si>
   <si>
     <t>FECHA_ACTIVIDAD</t>
+  </si>
+  <si>
+    <t>HORAS_ACTIVIDAD</t>
+  </si>
+  <si>
+    <t>RESERVA_ID</t>
+  </si>
+  <si>
+    <t>usario_id de reservas null== de administracion</t>
+  </si>
+  <si>
+    <t>HORAS_ACTIVIDAD_ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -279,16 +298,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -413,87 +445,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -502,33 +458,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -538,22 +485,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -565,7 +506,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -841,34 +818,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:K47"/>
+  <dimension ref="A4:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="18.44140625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
     <col min="7" max="7" width="18.44140625" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" customWidth="1"/>
     <col min="9" max="9" width="18.44140625" customWidth="1"/>
     <col min="10" max="10" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:11">
-      <c r="B5" s="44" t="s">
+    <row r="4" spans="1:11" ht="15" thickBot="1"/>
+    <row r="5" spans="1:11" ht="15" thickBot="1">
+      <c r="B5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="G5" s="35" t="s">
+      <c r="C5" s="34"/>
+      <c r="D5" s="35"/>
+      <c r="G5" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="36"/>
-      <c r="I5" s="37"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="35"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
@@ -1007,79 +985,82 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="G13" s="5" t="s">
+      <c r="D13" s="7"/>
+      <c r="G13" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I13" s="7" t="s">
+      <c r="H13" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="42" t="s">
+      <c r="J13" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="43"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="B14" s="47" t="s">
+      <c r="K13" s="32"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" thickBot="1">
+      <c r="B14" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="D14" s="11"/>
+      <c r="G14" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="I14" s="23" t="s">
+      <c r="H14" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="42"/>
-      <c r="K14" s="43"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="H15" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" s="24" t="s">
+      <c r="H15" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="42"/>
-      <c r="K15" s="43"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1">
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="36" t="s">
         <v>10</v>
       </c>
+      <c r="I16" s="38"/>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1">
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37"/>
-      <c r="G17" s="26" t="s">
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="G17" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="H17" s="26" t="s">
+      <c r="H17" s="40" t="s">
         <v>10</v>
       </c>
+      <c r="I17" s="41"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" t="s">
@@ -1105,11 +1086,11 @@
       <c r="D19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="35" t="s">
+      <c r="H19" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="I19" s="36"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="B20" s="5" t="s">
@@ -1149,30 +1130,30 @@
       <c r="J21" s="7"/>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="H22" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I22" s="15" t="s">
         <v>8</v>
       </c>
       <c r="J22" s="11"/>
     </row>
     <row r="24" spans="1:10" ht="15" thickBot="1"/>
     <row r="25" spans="1:10" ht="15" thickBot="1">
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="37"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="28"/>
     </row>
     <row r="26" spans="1:10" ht="15" thickBot="1">
       <c r="A26" t="s">
@@ -1187,11 +1168,11 @@
       <c r="D26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="44" t="s">
+      <c r="H26" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="I26" s="45"/>
-      <c r="J26" s="46"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="35"/>
     </row>
     <row r="27" spans="1:10">
       <c r="B27" s="5" t="s">
@@ -1269,10 +1250,10 @@
       <c r="J30" s="7"/>
     </row>
     <row r="31" spans="1:10" ht="15" thickBot="1">
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D31" s="11" t="s">
@@ -1296,22 +1277,22 @@
       <c r="J32" s="7"/>
     </row>
     <row r="33" spans="1:10" ht="15" thickBot="1">
-      <c r="H33" s="18" t="s">
+      <c r="H33" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="I33" s="13" t="s">
+      <c r="I33" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J33" s="23" t="s">
+      <c r="J33" s="21" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" thickBot="1">
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="37"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="35"/>
       <c r="H34" s="5" t="s">
         <v>25</v>
       </c>
@@ -1326,13 +1307,13 @@
       <c r="A35" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="7" t="s">
+      <c r="C35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H35" s="9" t="s">
@@ -1375,11 +1356,11 @@
       <c r="D38" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H38" s="38" t="s">
+      <c r="H38" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="I38" s="39"/>
-      <c r="J38" s="40"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="44"/>
     </row>
     <row r="39" spans="1:10">
       <c r="B39" s="5" t="s">
@@ -1389,14 +1370,17 @@
         <v>8</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="F39" s="27"/>
-      <c r="H39" s="19" t="s">
+      <c r="F39" s="24"/>
+      <c r="G39" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="H39" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="I39" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="J39" s="25" t="s">
+      <c r="I39" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="J39" s="23" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1408,17 +1392,18 @@
         <v>8</v>
       </c>
       <c r="D40" s="7"/>
-      <c r="H40" s="28" t="s">
+      <c r="G40" s="47"/>
+      <c r="H40" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="I40" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="J40" s="30" t="s">
+      <c r="I40" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="J40" s="59" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15" thickBot="1">
+    <row r="41" spans="1:10">
       <c r="B41" s="5" t="s">
         <v>57</v>
       </c>
@@ -1426,15 +1411,15 @@
         <v>8</v>
       </c>
       <c r="D41" s="7"/>
-      <c r="H41" s="31" t="s">
+      <c r="H41" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="I41" s="32" t="s">
+      <c r="I41" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="J41" s="33"/>
-    </row>
-    <row r="42" spans="1:10">
+      <c r="J41" s="38"/>
+    </row>
+    <row r="42" spans="1:10" ht="15" thickBot="1">
       <c r="B42" s="5" t="s">
         <v>58</v>
       </c>
@@ -1442,72 +1427,175 @@
         <v>8</v>
       </c>
       <c r="D42" s="7"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="22"/>
-      <c r="J42" s="22"/>
+      <c r="G42" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="H42" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="I42" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="J42" s="60"/>
     </row>
     <row r="43" spans="1:10" ht="15" thickBot="1">
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D43" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="D43" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
     </row>
     <row r="44" spans="1:10" ht="15" thickBot="1">
-      <c r="B44" s="34" t="s">
+      <c r="B44" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="34" t="s">
+      <c r="C44" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="H44" s="41" t="s">
+      <c r="D44" s="11"/>
+      <c r="H44" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="I44" s="39"/>
-      <c r="J44" s="40"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="30"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="H45" s="19" t="s">
+      <c r="G45" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="H45" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="I45" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="J45" s="25" t="s">
+      <c r="I45" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="J45" s="23" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:10">
-      <c r="H46" s="18" t="s">
+      <c r="G46" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="H46" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I46" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="J46" s="23" t="s">
+      <c r="I46" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J46" s="21" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" thickBot="1">
-      <c r="H47" s="21" t="s">
+      <c r="H47" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I47" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J47" s="24" t="s">
+      <c r="I47" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="J47" s="22" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="48" spans="1:10" ht="15" thickBot="1">
+      <c r="B48" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="49"/>
+      <c r="D48" s="50"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="47"/>
+      <c r="B49" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="B50" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="47"/>
+      <c r="B51" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="E51" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="B52" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" s="53"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="B54" s="51"/>
+      <c r="C54" s="52"/>
+      <c r="D54" s="53"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="B55" s="51"/>
+      <c r="C55" s="52"/>
+      <c r="D55" s="53"/>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="B56" s="51"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="53"/>
+    </row>
+    <row r="57" spans="1:5" ht="15" thickBot="1">
+      <c r="B57" s="54"/>
+      <c r="C57" s="55"/>
+      <c r="D57" s="56"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="B48:D48"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="H38:J38"/>
     <mergeCell ref="H44:J44"/>

</xml_diff>

<commit_message>
BBDD fecha fin actividad
</commit_message>
<xml_diff>
--- a/CentroDeportivo/DDBB/IPS BD RELACIONAL.xlsx
+++ b/CentroDeportivo/DDBB/IPS BD RELACIONAL.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="73">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>Cancelada se mira en reserva</t>
+  </si>
+  <si>
+    <t>fECHA_ACTIVIDAD_FIN</t>
+  </si>
+  <si>
+    <t>FECHA_ACTIVIDAD_INICIO</t>
   </si>
 </sst>
 </file>
@@ -362,7 +368,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -484,26 +490,6 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -516,22 +502,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -586,13 +561,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -641,10 +617,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -922,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -940,16 +912,16 @@
   <sheetData>
     <row r="4" spans="1:11" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:11" ht="15.75" thickBot="1">
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="63"/>
-      <c r="G5" s="61" t="s">
+      <c r="C5" s="63"/>
+      <c r="D5" s="64"/>
+      <c r="G5" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="62"/>
-      <c r="I5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="64"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
@@ -1018,7 +990,7 @@
       <c r="C9" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D9" s="56" t="s">
         <v>68</v>
       </c>
       <c r="E9" t="s">
@@ -1041,7 +1013,7 @@
       <c r="C10" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="58" t="s">
+      <c r="D10" s="56" t="s">
         <v>68</v>
       </c>
       <c r="G10" s="5" t="s">
@@ -1055,10 +1027,10 @@
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="55" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="53"/>
@@ -1117,32 +1089,32 @@
         <v>10</v>
       </c>
       <c r="D14" s="48"/>
-      <c r="G14" s="78" t="s">
+      <c r="G14" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="H14" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="I14" s="80" t="s">
+      <c r="H14" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="J14" s="76" t="s">
+      <c r="J14" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="K14" s="76"/>
+      <c r="K14" s="77"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="G15" s="78" t="s">
+      <c r="G15" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" s="80" t="s">
+      <c r="H15" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="J15" s="76"/>
-      <c r="K15" s="76"/>
+      <c r="J15" s="77"/>
+      <c r="K15" s="77"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1">
       <c r="G16" s="26" t="s">
@@ -1152,15 +1124,15 @@
         <v>10</v>
       </c>
       <c r="I16" s="27"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="76"/>
+      <c r="J16" s="77"/>
+      <c r="K16" s="77"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="65"/>
-      <c r="D17" s="66"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="67"/>
       <c r="G17" s="28" t="s">
         <v>62</v>
       </c>
@@ -1193,11 +1165,11 @@
       <c r="D19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="64" t="s">
+      <c r="H19" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="I19" s="65"/>
-      <c r="J19" s="66"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="67"/>
     </row>
     <row r="20" spans="1:10">
       <c r="B20" s="5" t="s">
@@ -1256,11 +1228,11 @@
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="25" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="65"/>
-      <c r="D25" s="66"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="67"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" thickBot="1">
       <c r="A26" t="s">
@@ -1275,11 +1247,11 @@
       <c r="D26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="61" t="s">
+      <c r="H26" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="I26" s="62"/>
-      <c r="J26" s="63"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="64"/>
     </row>
     <row r="27" spans="1:10">
       <c r="B27" s="5" t="s">
@@ -1395,11 +1367,11 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B34" s="61" t="s">
+      <c r="B34" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="62"/>
-      <c r="D34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="64"/>
       <c r="H34" s="5" t="s">
         <v>25</v>
       </c>
@@ -1463,11 +1435,11 @@
       <c r="D38" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H38" s="70" t="s">
+      <c r="H38" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="I38" s="71"/>
-      <c r="J38" s="72"/>
+      <c r="I38" s="72"/>
+      <c r="J38" s="73"/>
     </row>
     <row r="39" spans="1:10">
       <c r="B39" s="5" t="s">
@@ -1567,11 +1539,11 @@
         <v>44</v>
       </c>
       <c r="D44" s="11"/>
-      <c r="H44" s="73" t="s">
+      <c r="H44" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="I44" s="74"/>
-      <c r="J44" s="75"/>
+      <c r="I44" s="75"/>
+      <c r="J44" s="76"/>
     </row>
     <row r="45" spans="1:10">
       <c r="G45" s="33" t="s">
@@ -1613,11 +1585,11 @@
       </c>
     </row>
     <row r="48" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B48" s="67" t="s">
+      <c r="B48" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="C48" s="68"/>
-      <c r="D48" s="69"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="70"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="33"/>
@@ -1643,7 +1615,7 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="77" t="s">
+      <c r="A51" s="58" t="s">
         <v>2</v>
       </c>
       <c r="B51" s="34" t="s">
@@ -1680,7 +1652,7 @@
     </row>
     <row r="54" spans="1:5">
       <c r="B54" s="34" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C54" s="35" t="s">
         <v>10</v>
@@ -1701,19 +1673,25 @@
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="59"/>
+      <c r="A56" s="57"/>
       <c r="B56" s="49" t="s">
         <v>13</v>
       </c>
       <c r="C56" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="D56" s="59"/>
-    </row>
-    <row r="57" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B57" s="54"/>
-      <c r="C57" s="55"/>
-      <c r="D57" s="60"/>
+      <c r="D56" s="57"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="B57" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="36" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>